<commit_message>
Add new selection for term tree
</commit_message>
<xml_diff>
--- a/public/pdf/TreeTermTwo.xlsx
+++ b/public/pdf/TreeTermTwo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mick-Labtop\Desktop\Web\table-time\public\pdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mickz\OneDrive\เดสก์ท็อป\WEB Project\tabletime\public\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C6E8B2-B198-4A75-8115-2707AEFAE5CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093D80EC-C37F-433C-9C79-196E964B8DA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672" xr2:uid="{7148176E-7B6F-4397-9CFA-81A45D434018}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9675" xr2:uid="{7148176E-7B6F-4397-9CFA-81A45D434018}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>คาบที่</t>
   </si>
@@ -87,12 +87,6 @@
     <t>ประสบการณ์การทำงานทางวิชาชีพ</t>
   </si>
   <si>
-    <t>หัวข้อพิเศษทางเทคโนโลยีดิจิทัลคอนเทนต์ CS3</t>
-  </si>
-  <si>
-    <t>หัวข้อพิเศษทางเทคโนโลยีดิจิทัลคอนเทนต์ CS2</t>
-  </si>
-  <si>
     <t>อินเทอร์เน็ตประสานสรรพสิ่ง CS7</t>
   </si>
   <si>
@@ -100,6 +94,9 @@
   </si>
   <si>
     <t>กฎหมายและจริยธรรมทางเทคโนโลยีสารสนเทศ ห้อง 921</t>
+  </si>
+  <si>
+    <t>การถ่ายภาพเพื่องานออกแบบดิจิทัลคอนเทนต์</t>
   </si>
 </sst>
 </file>
@@ -139,7 +136,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,8 +167,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -209,17 +212,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -235,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -243,69 +235,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -329,7 +297,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -628,15 +596,15 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="10.77734375" customWidth="1"/>
+    <col min="1" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -674,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -712,126 +680,122 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="G3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="16"/>
+      <c r="L4" s="9"/>
     </row>
-    <row r="5" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="9"/>
+      <c r="B6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="19"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="F7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="5"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:J4"/>
+  <mergeCells count="15">
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="B5:D5"/>
@@ -840,6 +804,13 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.3" top="0.2" bottom="0.2" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Change PDF to PNG
</commit_message>
<xml_diff>
--- a/public/pdf/TreeTermTwo.xlsx
+++ b/public/pdf/TreeTermTwo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mickz\OneDrive\เดสก์ท็อป\WEB Project\tabletime\public\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093D80EC-C37F-433C-9C79-196E964B8DA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AC338-BAB2-4237-A8B6-612000AD6130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9675" xr2:uid="{7148176E-7B6F-4397-9CFA-81A45D434018}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>คาบที่</t>
   </si>
@@ -96,7 +96,7 @@
     <t>กฎหมายและจริยธรรมทางเทคโนโลยีสารสนเทศ ห้อง 921</t>
   </si>
   <si>
-    <t>การถ่ายภาพเพื่องานออกแบบดิจิทัลคอนเทนต์</t>
+    <t>หัวข้อพิเศษทางเทคโนโลยีดิจิทัลคอนเทนต์ CS3</t>
   </si>
 </sst>
 </file>
@@ -174,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -197,37 +197,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,38 +212,32 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +564,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,12 +661,12 @@
         <v>19</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="7"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="3" t="s">
         <v>19</v>
       </c>
@@ -708,21 +676,21 @@
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
       <c r="K4" s="9" t="s">
         <v>21</v>
       </c>
@@ -752,50 +720,54 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="11" t="s">
+      <c r="J6" s="8"/>
+      <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="11"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G3:J3"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="B5:D5"/>
@@ -804,13 +776,6 @@
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="F6:H6"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.3" top="0.2" bottom="0.2" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>